<commit_message>
improvements on the notebook
</commit_message>
<xml_diff>
--- a/data/performance_table.xlsx
+++ b/data/performance_table.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,10 +418,10 @@
         <v>Annthyroid</v>
       </c>
       <c r="B2" t="str">
-        <v>0.11314</v>
+        <v>0.0593</v>
       </c>
       <c r="C2" t="str">
-        <v>0.0906</v>
+        <v>0.1967</v>
       </c>
     </row>
     <row r="3">
@@ -429,15 +429,235 @@
         <v>Arrhythmia</v>
       </c>
       <c r="B3" t="str">
-        <v>0.09884</v>
+        <v>0.1753</v>
       </c>
       <c r="C3" t="str">
-        <v>0.0745</v>
+        <v>0.3798</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Breastw</v>
+      </c>
+      <c r="B4" t="str">
+        <v>0.6431</v>
+      </c>
+      <c r="C4" t="str">
+        <v>0.3453</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Glass</v>
+      </c>
+      <c r="B5" t="str">
+        <v>0.0411</v>
+      </c>
+      <c r="C5" t="str">
+        <v>0.1092</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Ionosphere</v>
+      </c>
+      <c r="B6" t="str">
+        <v>0.7711</v>
+      </c>
+      <c r="C6" t="str">
+        <v>0.8635</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Letter</v>
+      </c>
+      <c r="B7" t="str">
+        <v>0.113</v>
+      </c>
+      <c r="C7" t="str">
+        <v>0.2714</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Lympho</v>
+      </c>
+      <c r="B8" t="str">
+        <v>0.2946</v>
+      </c>
+      <c r="C8" t="str">
+        <v>0.8012</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Mammography</v>
+      </c>
+      <c r="B9" t="str">
+        <v>0.1886</v>
+      </c>
+      <c r="C9" t="str">
+        <v>0.1381</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Mnist</v>
+      </c>
+      <c r="B10" t="str">
+        <v>0.107</v>
+      </c>
+      <c r="C10" t="str">
+        <v>0.3401</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Musk</v>
+      </c>
+      <c r="B11" t="str">
+        <v>0.138</v>
+      </c>
+      <c r="C11" t="str">
+        <v>0.0836</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Optdigits</v>
+      </c>
+      <c r="B12" t="str">
+        <v>0.0172</v>
+      </c>
+      <c r="C12" t="str">
+        <v>0.0222</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Pendigits</v>
+      </c>
+      <c r="B13" t="str">
+        <v>0.1309</v>
+      </c>
+      <c r="C13" t="str">
+        <v>0.0282</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Pima</v>
+      </c>
+      <c r="B14" t="str">
+        <v>0.5441</v>
+      </c>
+      <c r="C14" t="str">
+        <v>0.4686</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Satellite</v>
+      </c>
+      <c r="B15" t="str">
+        <v>0.2217</v>
+      </c>
+      <c r="C15" t="str">
+        <v>0.3958</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>SatImage-2</v>
+      </c>
+      <c r="B16" t="str">
+        <v>0.5139</v>
+      </c>
+      <c r="C16" t="str">
+        <v>0.0422</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Shuttle</v>
+      </c>
+      <c r="B17" t="str">
+        <v>0.4371</v>
+      </c>
+      <c r="C17" t="str">
+        <v>0.123</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Speech</v>
+      </c>
+      <c r="B18" t="str">
+        <v>0.0184</v>
+      </c>
+      <c r="C18" t="str">
+        <v>0.0194</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Thyroid</v>
+      </c>
+      <c r="B19" t="str">
+        <v>0.0151</v>
+      </c>
+      <c r="C19" t="str">
+        <v>0.2832</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Vertebral</v>
+      </c>
+      <c r="B20" t="str">
+        <v>0.0886</v>
+      </c>
+      <c r="C20" t="str">
+        <v>0.0847</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Vowels</v>
+      </c>
+      <c r="B21" t="str">
+        <v>0.0274</v>
+      </c>
+      <c r="C21" t="str">
+        <v>0.4071</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Wbc</v>
+      </c>
+      <c r="B22" t="str">
+        <v>0.4221</v>
+      </c>
+      <c r="C22" t="str">
+        <v>0.5965</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Wine</v>
+      </c>
+      <c r="B23" t="str">
+        <v>0.633</v>
+      </c>
+      <c r="C23" t="str">
+        <v>0.3367</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>